<commit_message>
api config final test
</commit_message>
<xml_diff>
--- a/R1Contact/src/test/resources/TestData/ApiConfigutationData.xlsx
+++ b/R1Contact/src/test/resources/TestData/ApiConfigutationData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="166925"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21945" windowHeight="4425"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15915" windowHeight="3720" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="WHEATON FRANCISCAN HEALTHCARE" sheetId="1" r:id="rId1"/>
@@ -14,23 +14,17 @@
     <sheet name="CRITTENTON HOSPITAL" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:L12"/>
+  <oleSize ref="A1:H10"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="67">
   <si>
     <t>Vendor</t>
   </si>
@@ -198,13 +192,46 @@
   </si>
   <si>
     <t>https://crittenton-api.webview.com/admin/document</t>
+  </si>
+  <si>
+    <t>LKMN</t>
+  </si>
+  <si>
+    <t>Test1</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Test2wqeqwe</t>
+  </si>
+  <si>
+    <t>Test3</t>
+  </si>
+  <si>
+    <t>Test4</t>
+  </si>
+  <si>
+    <t>Connector</t>
+  </si>
+  <si>
+    <t>merge</t>
+  </si>
+  <si>
+    <t>LKNJ</t>
+  </si>
+  <si>
+    <t>AHI053</t>
+  </si>
+  <si>
+    <t>https://lourdesnet-api.webview.com/admin/document</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,8 +247,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF676767"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -231,6 +264,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8F8F8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -262,7 +307,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -270,6 +315,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,12 +650,12 @@
     <col min="5" max="5" width="36.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
     <col min="9" max="9" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -634,7 +687,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -656,8 +709,8 @@
       <c r="G2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>15</v>
+      <c r="H2" s="7">
+        <v>55101</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>12</v>
@@ -666,7 +719,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -688,8 +741,8 @@
       <c r="G3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>15</v>
+      <c r="H3" s="7">
+        <v>55101</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>12</v>
@@ -698,7 +751,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -720,8 +773,8 @@
       <c r="G4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>15</v>
+      <c r="H4" s="7">
+        <v>55101</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>12</v>
@@ -730,7 +783,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -752,8 +805,8 @@
       <c r="G5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>15</v>
+      <c r="H5" s="7">
+        <v>55101</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>12</v>
@@ -762,7 +815,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
@@ -784,8 +837,8 @@
       <c r="G6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>15</v>
+      <c r="H6" s="7">
+        <v>55101</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>12</v>
@@ -794,7 +847,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -816,8 +869,8 @@
       <c r="G7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>15</v>
+      <c r="H7" s="7">
+        <v>55101</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>12</v>
@@ -826,7 +879,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -848,8 +901,8 @@
       <c r="G8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>15</v>
+      <c r="H8" s="7">
+        <v>55101</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>12</v>
@@ -858,6 +911,30 @@
         <v>17</v>
       </c>
     </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="8:12" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="8:12" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="8:12" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="8:12" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="8:12" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="8:12" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="8:12" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="8:12" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="8:12" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="8:12" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="8:12" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="8:12" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="8:12" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="8:12" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="8:12" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="8:12" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -869,7 +946,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -937,8 +1014,8 @@
       <c r="G2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="6">
-        <v>47238</v>
+      <c r="H2" s="7">
+        <v>55101</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>31</v>
@@ -969,8 +1046,8 @@
       <c r="G3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="6">
-        <v>47238</v>
+      <c r="H3" s="7">
+        <v>55101</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>31</v>
@@ -1001,8 +1078,8 @@
       <c r="G4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="6">
-        <v>47238</v>
+      <c r="H4" s="7">
+        <v>55101</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>31</v>
@@ -1033,8 +1110,8 @@
       <c r="G5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="6">
-        <v>47238</v>
+      <c r="H5" s="7">
+        <v>55101</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>31</v>
@@ -1065,8 +1142,8 @@
       <c r="G6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="6">
-        <v>47238</v>
+      <c r="H6" s="7">
+        <v>55101</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>31</v>
@@ -1097,8 +1174,8 @@
       <c r="G7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="6">
-        <v>47238</v>
+      <c r="H7" s="7">
+        <v>55101</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>31</v>
@@ -1129,8 +1206,8 @@
       <c r="G8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="6">
-        <v>47238</v>
+      <c r="H8" s="7">
+        <v>55101</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>31</v>
@@ -1161,8 +1238,8 @@
       <c r="G9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="6">
-        <v>47238</v>
+      <c r="H9" s="7">
+        <v>55101</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>31</v>
@@ -1193,8 +1270,8 @@
       <c r="G10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="6">
-        <v>47238</v>
+      <c r="H10" s="7">
+        <v>55101</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>31</v>
@@ -1225,8 +1302,8 @@
       <c r="G11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="6">
-        <v>47238</v>
+      <c r="H11" s="7">
+        <v>55101</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>42</v>
@@ -1237,15 +1314,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1255,6 +1333,7 @@
     <col min="4" max="4" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
     <col min="9" max="9" width="60.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
   </cols>
@@ -1313,8 +1392,8 @@
       <c r="G2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="6">
-        <v>47238</v>
+      <c r="H2" s="7">
+        <v>55101</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>44</v>
@@ -1345,8 +1424,8 @@
       <c r="G3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="6">
-        <v>47238</v>
+      <c r="H3" s="7">
+        <v>55101</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>44</v>
@@ -1377,8 +1456,8 @@
       <c r="G4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="6">
-        <v>47238</v>
+      <c r="H4" s="7">
+        <v>55101</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>44</v>
@@ -1409,8 +1488,8 @@
       <c r="G5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="6">
-        <v>47238</v>
+      <c r="H5" s="7">
+        <v>55101</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>44</v>
@@ -1441,8 +1520,8 @@
       <c r="G6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="6">
-        <v>47238</v>
+      <c r="H6" s="7">
+        <v>55101</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>44</v>
@@ -1473,13 +1552,45 @@
       <c r="G7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="6">
-        <v>47238</v>
+      <c r="H7" s="7">
+        <v>55101</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>44</v>
       </c>
       <c r="J7" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="H8" s="7">
+        <v>55101</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="J8" s="3" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1490,10 +1601,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1501,8 +1612,9 @@
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="51.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.7109375" customWidth="1"/>
+    <col min="6" max="6" width="26" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1"/>
     <col min="9" max="9" width="56.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
   </cols>
@@ -1561,8 +1673,8 @@
       <c r="G2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="6">
-        <v>47238</v>
+      <c r="H2" s="7">
+        <v>55101</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>53</v>
@@ -1593,8 +1705,8 @@
       <c r="G3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="6">
-        <v>47238</v>
+      <c r="H3" s="7">
+        <v>55101</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>53</v>
@@ -1625,8 +1737,8 @@
       <c r="G4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="6">
-        <v>47238</v>
+      <c r="H4" s="7">
+        <v>55101</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>53</v>
@@ -1635,7 +1747,42 @@
         <v>32</v>
       </c>
     </row>
+    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="7">
+        <v>55101</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I5" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>